<commit_message>
Latest data: Fri Aug 26 09:23:12 UTC 2022
</commit_message>
<xml_diff>
--- a/data_final.xlsx
+++ b/data_final.xlsx
@@ -16,14 +16,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +48,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +429,696 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>JobId</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>CollectedDate</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>JobTitle</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CompanyName</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>RatingNumber</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>PostedDate</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Salary</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>jobType</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>JobURL</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ShortDiscribtion</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>fullJobDescribtion</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Posted_Date_N</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Marseille</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1008093549599</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>44799</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Data Analyst H/F</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>RHODANIENNE DE TRANSIT</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>24h</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1136043&amp;s=58&amp;guid=00000182d974ed8d8a401d24b0b448bd&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;ea=1&amp;cs=1_fbf630ed&amp;cb=1661505695437&amp;jobListingId=1008093549599&amp;jrtk=3-0-1gbcn9rdmghp0801-1gbcn9re9jm5f800-205871229e3be2d4-</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Chef d’orchestre du transport international, le Groupe RDT organise la logistique et le transport de marchandises à travers le monde.
+Chaque jour, nous nous attachons à fournir un service de qualité en plaçant le client au centre de notre activité.
+Dans le cadre de notre développement, nous proposons un poste de Data Analyst en alternance.
+Rattaché(e) au Directeur Administratif et Financier du groupe basé au siège à Marseille, vous aurez le rôle de mieux comprendre les données financières afin d’en tirer des informations de grande valeur pour l’entreprise.
+Vos missions seront de :
+Créer et interroger des bases de données afin de récupérer les données pertinentes,
+Créer des dashboards comprenant des graphiques et indicateurs pertinents,
+Collecter, préparer et fiabiliser les données en vue de vos analyses,
+Mettre en place des outils de contrôle de cohérence sur les données,
+Rédiger, et mettre en place des procédures et modes opératoires,
+Mettre en place des outils de pilotage financier, KPI.
+Votre profil :
+Issu(e) d’une formation de type Licence ou Master en DATA, Finance ou Contrôle de gestion, vous justifiez d’une appétence pour l’analyse de données et le Big Data.
+Vous aimez les chiffres et maitrisez Excel ainsi que le langage SQL ?
+Vous êtes dynamique, rigoureux(se) et motivé(e) avec le sens des initiatives ?
+N’attendez plus et rejoignez une équipe en plein développement !
+Type d'emploi : Alternance
+Avantages :
+Horaires flexibles
+Titre-restaurant
+Programmation :
+Du Lundi au Vendredi
+Périodes de travail de 8 heures
+Types de primes et de gratifications :
+13ème Mois</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>44775</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Bordeaux</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1008085342780</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>44799</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Data scientist H/F</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Unicancer
+3.0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>3d</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>€37K (Employer est.)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1136043&amp;s=58&amp;guid=00000182d974ed8d8a401d24b0b448bd&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;cs=1_03dd6d0b&amp;cb=1661505695438&amp;jobListingId=1008085342780&amp;jrtk=3-0-1gbcn9rdmghp0801-1gbcn9re9jm5f800-6b05d241bacc3752-</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Mission principale :
+Au sein de l’unité de recherche et de surveillance épidémiologique du Centre de Lutte Contre le Cancer Bordelais (Institut Bergonié, INSERM U1219).
+Cette équipe a la gestion du registre des Hémopathies Malignes de la Gironde (surveillance épidémiologique des lymphomes et leucémies), de la partie épidémiologique de la cohorte REALYSA (recherche étiologique et pronostic des lymphomes en France) et du projet GEO-K-PHYTO (Exposition aux pesticides et hémopathies malignes).
+Vous travaillez sur ce dernier projet dont l’objectif principal vise à soutenir des pouvoirs publics dans le but d’améliorer les connaissances sur l’impact sanitaire des produits phytopharmaceutiques. Pour se faire, nous mettons en place le premier dispositif de surveillance épidémiologique des cancers de l’adulte (15 ans et plus) vivant à proximité de zones agricoles avec une méthodologie avancée sur la caractérisation des expositions.
+Data scientist H/F
+Missions
+Activités générales :
+Sous la responsabilité du statisticien de l’unité, vous aurez pour mission de conduire la suite du projet GEO-K-PHYTO en ce qui concerne les tâches suivantes :
+Mise en place de l’analyse sur 8 départements couverts par l’étude :
+Vous vérifiez de la qualité des données ;
+Vous accédez aux données INSEE pour appariement (étude CAS/TEMOINS) ;
+Vous menez la réalisation des analyses statistiques dans le système sécurisé de la structure INSEE.
+Rédaction du rapport d’analyse :
+Vous détaillez la méthode d’analyse utilisée ;
+Vous menez la rédaction de documents structurés (analyse descriptive, modélisation…).
+Propositions de développements méthodologiques :
+Vous mettez en œuvre de modèles statistique sophistiqués en complément des analyses déjà réalisées ;
+Coordination du projet entre les différents partenaires :
+Vous établissez le transfert et le recueil des données registres de cancer ;
+Vous animez des réunions.
+Profil
+Profil attendu :
+Vous avez suivi une solide formation en analyse statistiques (Ingénieur ENSAI) : BAC +5 ou plus ;
+Vous avez également des capacités rédactionnelles Français/Anglais.
+Compétences requises :
+Vous connaissez le logiciel R (procédures de nettoyage des bases de données : données manquantes, vérification des incohérences, statistiques descriptives) ;
+Vous connaissez le langage SQL et python ;
+Vous connaissez le SIG et l’analyse géographique ;
+Vous avez de bonnes capacités de synthèse ;
+Vous faites preuve de méthode et rigueur ;
+Vous savez travailler en équipe.
+Atouts du poste :
+Accessibilité et transports :
+L’Institut est desservi par les transports en commun : Tram B ; Bus lignes 5, 26, 9.
+Par ailleurs, des places de parking sont prévues pour les personnes à mobilité réduite. Un parking vélo est également à disposition ;
+La prise en charge de l’abonnement transport en commun à 60% ;
+Comité Social et Économique : chèques cadeaux, chèques rentrée scolaire, places de cinéma… ;
+Une restauration collective avec tarif préférentiel (3,26€)
+Plage horaire :Jours travaillés sont du lundi au vendredi et horaires de journée.
+Durée :Contrat à Durée Déterminée : 12 mois
+Rémunération : Catégorie Cadre Niv.1 selon grille de rémunération des CLCC, 3118,58€ bruts/mois en temps plein.</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lille</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1008088346396</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>44799</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Data Analyst Junior (H/F)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Insitoo
+5.0</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2d</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1136043&amp;s=58&amp;guid=00000182d974ed8d8a401d24b0b448bd&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;cs=1_0c4f1c32&amp;cb=1661505695438&amp;jobListingId=1008088346396&amp;jrtk=3-0-1gbcn9rdmghp0801-1gbcn9re9jm5f800-06fbc509f0553b7d-</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Basée à Lille, Lyon, Nantes, Grenoble et Bruxelles, Insitoo Freelances est une société du groupe Insitoo, spécialisée dans le placement et le sourcing des Freelances IT et Métier. Depuis 2007, Insitoo Freelances a su s’imposer comme une référence en matière de freelancing par son expertise dans l’IT et ses valeurs de transparence et de proximité. Actuellement, afin de répondre aux besoins de nos clients, nous recherchons un Data Analyst Junior (H/F) à Lille, Hauts-de-France, France.
+Nous recherchons un data Analyst junior, il intégrera l’équipe Trafic et analytics de la Direction Ecommerce.
+La direction ecommerce a de fortes ambitions sur le digital sur la fin d’année et à pour ambition de mieux comprendre et exploiter ces données afin de prendre les bonnes décisions et de mesurer les impacts des évolutions sur le site. (Optimisation de campagne, amélioration produits …).
+Les missions attendues par le Data Analyst Junior (H/F) sont :
+Explorer, exploiter et interpréter les données afin de faire des analyses poussées conduisant à améliorer la performance digitale (Media digitaux, UX, campagnes monétisation, CRM, e-merchandising, animation commerciale web).
+Etre capable de prendre de la hauteur sur les différents socles de données afin d’en ressortir des recommandations et des analyses fines.
+Echanger avec les différents métiers sur les ‘pains’ rencontrés.
+Challenger les besoins et creuser les réflexions.
+Proposer des analyses adéquates et des recommandations.
+Travailler sur des dashboards complexes afin de faciliter la vie des métiers.
+Le data analyse recherché doit avoir des compétences suivantes :
+– Big Query
+– SQL
+– DataStudio
+Cette mission vous intéresse?
+Vous justifiez d’une expérience significative comme Data Analyst Junior (H/F) ?
+Vous êtes rigoureux, méthodique, organisé et vous savez faire preuve d’autonomie et de réactivité ?
+Vous êtes à l’aise à l’écrit comme à l’oral ?
+Vous maîtrisez les périmètres techniques cités avec les niveaux adéquats ?
+Vous aimez évoluer dans un univers où l’autonomie, la prise d’initiatives, le partage et le travail en équipe sont porteurs de la réussite collective ?
+Vous pensez que votre profil pourrait correspondre au besoin de notre client ?
+N’attendez plus pour déposer votre candidature, nos Ingénieurs d’affaires se feront un plaisir de vous en dire plus !
+Référence : 07-JAUNE-QO</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>44797</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Qatar</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Doha</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1008090011376</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>44799</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Administration Officer</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Human Capital Group
+2.0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2d</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1136043&amp;s=58&amp;guid=00000182d975cb3ba54891f6f9725c8c&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;ea=1&amp;cs=1_994358c9&amp;cb=1661505752190&amp;jobListingId=1008090011376&amp;jrtk=3-0-1gbcnbirp2hs4001-1gbcnbisdghqi800-4c920122a36f3480-</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Job Description
+Manage and co-ordinate internal and external communications including handling all calls in efficient and professional manner.
+To act as first point of contact for incoming queries from external and internal stakeholders. To provide administrative support including answering phones, distributing post, word processing, preparation of PowerPoint presentations, drafting of letters, electronic communications, minute taking, setting up and maintaining excel spreadsheets, data input into databases, management of databases, file management, diaty management, photocopying, faxing, checking and responding to emails and any other related duties.
+Responsible for maintaining petty cash record and arrange for petty cash reimbursement .
+Responsible for generating business documentation, including but not limited to report writing, presentation creation and spread sheet preparation and distribution.
+Responsible in ensuring that the structure, standards, processed and tools as defined by the company are in place and maintained.
+To assist in the maintenance and delivery of policies and procedures in the areas of human resources, health and safety.
+To make travel and hotel accommodation arrangements in line with agreed guidelines and procedures. Responsible for supporting the Line Manager and the department in delivering planned projects within a specified deadline, in terms of documentation, follow-ups, task coordination.
+REQUIRED QUALIFICATIONS, KNOWLEDGE, SKILLS, AND EXPERIENCE
+1. Minimum Qualification:
+- min Diploma / Bachelor’s level or equivalent
+2. Minimum Experience:
+Minimum 4 years relevant working experience
+3. Job Specific Skills: Essential skills
+- Command of English language.
+- Excellent relationship and networking skills.
+- Strong decision making and problem-solving skills.
+- Highly computer literate in Microsoft Office (Word, Excel, Access, PowerPoint and Outlook)
+Ability to commute/relocate:
+Doha: Reliably commute or planning to relocate before starting work (Required)</t>
+        </is>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>44797</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Qatar</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Doha</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1008093382931</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>44799</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>DATA ENTRY OPERATOR</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Applynewjobs Consulting
+4.0</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>24h</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1136043&amp;s=58&amp;guid=00000182d975cb3ba54891f6f9725c8c&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;cs=1_74da42c9&amp;cb=1661505752190&amp;jobListingId=1008093382931&amp;jrtk=3-0-1gbcnbirp2hs4001-1gbcnbisdghqi800-469b6a7fae707b60-</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Published
+August 25, 2022
+Location
+Doha, Qatar
+Category
+Administration / Front Desk / PA / Secretary
+Job Type
+Full-time
+Description
+Looking for a Data Entry Operator for Doha, Qatar.
+Job Responsibilities:
+Entering data from source documents to system within time limits.
+Compiling, verifying the accuracy, and sorting information on the system.
+Research and obtain further information for incomplete documents.
+Respond to queries for information and access relevant files.
+Files and retrieves corporate documents, records, and reports.
+Reviewing data for deficiencies or errors, correcting any incompatibilities, and checking output.
+Job Requirements:
+High school Diploma.
+Two years experience as a Data entry operator.
+Trustworthy, able to respect confidentiality.
+Experience with MS Office and data programs.
+Demonstrates solid work ethics.</t>
+        </is>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>44775</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Qatar</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Doha</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1008082337071</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>44799</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Admin Coordinator</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Human Capital Group
+2.0</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>6d</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Full-time</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1136043&amp;s=58&amp;guid=00000182d975cb3ba54891f6f9725c8c&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;ea=1&amp;cs=1_9ed7fe65&amp;cb=1661505752190&amp;jobListingId=1008082337071&amp;jrtk=3-0-1gbcnbirp2hs4001-1gbcnbisdghqi800-14bfc531e60fd983-</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Performs various secretarial and administrative duties to support requirements and maintain the department functions smoothly on a daily basis.
+Handles a wide variety of situations and tasks involving the administrative function of the office. Tactfully handles enquiries and/or refer to appropriate personnel/department.
+Manages, coordinates and maintains calendar of appointments, travel arrangements, records of communication (documents, faxes, mail) to meet the requirements of the department, to record, filter, disseminate and communicate all incoming and outgoing matters.
+Provides business documentation support, including report writing, presentation creation and spreadsheet preparation and distribution of such materials. Compiles reports as directed and ensure that all files are complete and properly maintained.
+Independently manages multiple tasks and assigned projects whilst respecting the deadlines and simultaneously ensuring the integrity of all information and data.
+Communicates and provides information internally and externally to assist and enable administrative support and effective service to the concerned sections.
+REQUIRED QUALIFICATIONS, KNOWLEDGE, SKILLS, AND EXPERIENCE
+1. Minimum Qualification: - Min Diploma / Bachelor’s level or equivalent
+2. Minimum Experience: - Minimum 3 years relevant working experience
+3. Job Specific Skills: Essential skills -
+Ability to work in a cross culture environment.
+Excellent communication and computer skills.
+Excellent written/spoken English.
+Maintain confidentiality and self-discipline
+Job Type: Full-time
+Ability to commute/relocate:
+Doha: Reliably commute or planning to relocate before starting work (Required)</t>
+        </is>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>44793</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>